<commit_message>
Refactored exadata, added domain layer
</commit_message>
<xml_diff>
--- a/resources/templates/template_exadatas.xlsx
+++ b/resources/templates/template_exadatas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Memory-CPU" sheetId="1" state="visible" r:id="rId2"/>
@@ -57,13 +57,13 @@
     <t xml:space="preserve">vCPU Utilization [%]</t>
   </si>
   <si>
-    <t xml:space="preserve">Cell Raw [TB] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Used [TB]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usable Available [TB]</t>
+    <t xml:space="preserve">Cell Raw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Used</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usable Available</t>
   </si>
   <si>
     <t xml:space="preserve">Cluster</t>
@@ -249,8 +249,8 @@
   </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.34375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -306,7 +306,7 @@
   </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added reserved values to exadata export API
</commit_message>
<xml_diff>
--- a/resources/templates/template_exadatas.xlsx
+++ b/resources/templates/template_exadatas.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t xml:space="preserve">Exadata</t>
   </si>
@@ -45,6 +45,9 @@
     <t xml:space="preserve">Physical Memory used for VMs</t>
   </si>
   <si>
+    <t xml:space="preserve">Ram Reserved</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mem Utilization [%]</t>
   </si>
   <si>
@@ -52,6 +55,9 @@
   </si>
   <si>
     <t xml:space="preserve">vCPU used by VMs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vCPU Reserved</t>
   </si>
   <si>
     <t xml:space="preserve">vCPU Utilization [%]</t>
@@ -180,10 +186,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.34375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -193,10 +199,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="30.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="26.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="17.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="1" width="12.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -232,6 +238,12 @@
       </c>
       <c r="K1" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -258,7 +270,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.34375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="28.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22"/>
@@ -283,13 +295,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -308,7 +320,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
@@ -336,23 +348,20 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F2" s="0"/>
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>